<commit_message>
Updated PCK-CNC BOMs to match Assembly instructions
</commit_message>
<xml_diff>
--- a/BOMs/PCK CNC - BOM.xlsx
+++ b/BOMs/PCK CNC - BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pecka\Desktop\PCK-CNC\PCK-CNC\BOMs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B73C47C-3591-472F-97CC-EE79626FDFF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F6B6BB9-1E00-4E81-A9C6-3A7EF5379D58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{CE9F2058-9E2A-487E-A240-3F6A533D1330}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="212">
   <si>
     <t>Aluminum extrusions</t>
   </si>
@@ -154,12 +154,6 @@
   </si>
   <si>
     <t>Limit switch cables</t>
-  </si>
-  <si>
-    <t>Bolts &amp; Nuts</t>
-  </si>
-  <si>
-    <t>M3x5mm</t>
   </si>
   <si>
     <r>
@@ -363,51 +357,12 @@
     <t>Sourcing</t>
   </si>
   <si>
-    <t>M3x8mm</t>
-  </si>
-  <si>
-    <t>M3x10mm</t>
-  </si>
-  <si>
-    <t>M3x16mm</t>
-  </si>
-  <si>
-    <t>M2.5x16mm</t>
-  </si>
-  <si>
-    <t>M3x25mm</t>
-  </si>
-  <si>
-    <t>M4x8mm</t>
-  </si>
-  <si>
     <t>M3 T-Slot nut</t>
   </si>
   <si>
     <t>M4 T-Slot nut</t>
   </si>
   <si>
-    <t>M4x12mm</t>
-  </si>
-  <si>
-    <t>M4x16mm</t>
-  </si>
-  <si>
-    <t>M4x10mm</t>
-  </si>
-  <si>
-    <t>M4x20mm</t>
-  </si>
-  <si>
-    <t>M4 Insert</t>
-  </si>
-  <si>
-    <t>M3 Insert</t>
-  </si>
-  <si>
-    <t>M4x40mm</t>
-  </si>
-  <si>
     <t>M5 Nut</t>
   </si>
   <si>
@@ -417,27 +372,6 @@
     <t>M6 Nut</t>
   </si>
   <si>
-    <t>M6x70mm</t>
-  </si>
-  <si>
-    <t>M5x10mm</t>
-  </si>
-  <si>
-    <t>M5x8mm</t>
-  </si>
-  <si>
-    <t>M5x20mm</t>
-  </si>
-  <si>
-    <t>M5x25mm</t>
-  </si>
-  <si>
-    <t>M5x16mm</t>
-  </si>
-  <si>
-    <t>M5x50mm</t>
-  </si>
-  <si>
     <t>Length - 5mm</t>
   </si>
   <si>
@@ -774,13 +708,100 @@
     <t>230V 16A - 2NO</t>
   </si>
   <si>
-    <t>Flat head (Flat head)</t>
-  </si>
-  <si>
-    <t>Socket head (Socket head)</t>
-  </si>
-  <si>
-    <t>Pan head (Round head)</t>
+    <t>Screws &amp; nuts</t>
+  </si>
+  <si>
+    <t>M2.5x16 mm</t>
+  </si>
+  <si>
+    <t>M3x5 mm</t>
+  </si>
+  <si>
+    <t>M3x8 mm</t>
+  </si>
+  <si>
+    <t>M3x10 mm</t>
+  </si>
+  <si>
+    <t>M3x16 mm</t>
+  </si>
+  <si>
+    <t>M3x25 mm</t>
+  </si>
+  <si>
+    <t>M4x8 mm</t>
+  </si>
+  <si>
+    <t>M4x10 mm</t>
+  </si>
+  <si>
+    <t>M4x12 mm</t>
+  </si>
+  <si>
+    <t>M4x16 mm</t>
+  </si>
+  <si>
+    <t>M4x20 mm</t>
+  </si>
+  <si>
+    <t>M4x40 mm</t>
+  </si>
+  <si>
+    <t>M5x8 mm</t>
+  </si>
+  <si>
+    <t>M5x10 mm</t>
+  </si>
+  <si>
+    <t>M5x20 mm</t>
+  </si>
+  <si>
+    <t>M5x25 mm</t>
+  </si>
+  <si>
+    <t>M5x30 mm</t>
+  </si>
+  <si>
+    <t>M5x50 mm</t>
+  </si>
+  <si>
+    <t>M6x70 mm</t>
+  </si>
+  <si>
+    <t>3x20 mm wood screw</t>
+  </si>
+  <si>
+    <t>4x20 mm wood screw</t>
+  </si>
+  <si>
+    <t>M3 Nut</t>
+  </si>
+  <si>
+    <t>M4x6 mm</t>
+  </si>
+  <si>
+    <t>M3x20 mm</t>
+  </si>
+  <si>
+    <t>M4 Threaded insert</t>
+  </si>
+  <si>
+    <t>M3 Threaded insert</t>
+  </si>
+  <si>
+    <t>M3x12 mm</t>
+  </si>
+  <si>
+    <t>M2.5 Nut</t>
+  </si>
+  <si>
+    <t>Round head</t>
+  </si>
+  <si>
+    <t>Flat head</t>
+  </si>
+  <si>
+    <t>Socket head</t>
   </si>
 </sst>
 </file>
@@ -940,25 +961,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -967,12 +976,22 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hypertextový odkaz" xfId="1" builtinId="8"/>
@@ -1288,10 +1307,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1B021CE-7FB8-480D-A33D-38B9FC44AE4D}">
-  <dimension ref="A1:J161"/>
+  <dimension ref="A1:J169"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="J76" sqref="J76"/>
+    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
+      <selection activeCell="H89" sqref="H89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1304,12 +1323,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
@@ -1322,7 +1341,7 @@
         <v>2</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1333,9 +1352,9 @@
         <v>5</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="D3" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="14" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1347,57 +1366,57 @@
         <v>5</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D4" s="14"/>
+        <v>54</v>
+      </c>
+      <c r="D4" s="15"/>
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>1</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="D5" s="14"/>
+        <v>55</v>
+      </c>
+      <c r="D5" s="15"/>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>1</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D6" s="14"/>
+        <v>54</v>
+      </c>
+      <c r="D6" s="15"/>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>2</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="D7" s="14"/>
+        <v>56</v>
+      </c>
+      <c r="D7" s="15"/>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>2</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D8" s="10"/>
+        <v>57</v>
+      </c>
+      <c r="D8" s="16"/>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
@@ -1405,12 +1424,12 @@
       <c r="C9" s="1"/>
     </row>
     <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="18" t="s">
-        <v>113</v>
-      </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
+      <c r="A10" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
@@ -1423,7 +1442,7 @@
         <v>6</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1431,7 +1450,7 @@
         <v>2</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>8</v>
@@ -1445,7 +1464,7 @@
         <v>2</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>9</v>
@@ -1459,12 +1478,12 @@
         <v>1</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>114</v>
+        <v>92</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="D14" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="D14" s="9" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1473,34 +1492,34 @@
         <v>1</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>115</v>
+        <v>93</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="D15" s="12"/>
+        <v>99</v>
+      </c>
+      <c r="D15" s="11"/>
     </row>
     <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>1</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>116</v>
+        <v>94</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="D16" s="13"/>
+        <v>95</v>
+      </c>
+      <c r="D16" s="10"/>
     </row>
     <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>2</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>118</v>
+        <v>96</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>119</v>
+        <v>97</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>14</v>
@@ -1511,10 +1530,10 @@
         <v>2</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>118</v>
+        <v>96</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>120</v>
+        <v>98</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>14</v>
@@ -1525,10 +1544,10 @@
         <v>2</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>124</v>
+        <v>102</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>125</v>
+        <v>103</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>14</v>
@@ -1539,10 +1558,10 @@
         <v>1</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>123</v>
+        <v>101</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>126</v>
+        <v>104</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>14</v>
@@ -1550,12 +1569,12 @@
     </row>
     <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="19" t="s">
-        <v>112</v>
-      </c>
-      <c r="B22" s="19"/>
-      <c r="C22" s="19"/>
-      <c r="D22" s="19"/>
+      <c r="A22" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="B22" s="18"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
     </row>
     <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
@@ -1568,7 +1587,7 @@
         <v>6</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1579,9 +1598,9 @@
         <v>11</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="D24" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="D24" s="9" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1595,7 +1614,7 @@
       <c r="C25" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D25" s="13"/>
+      <c r="D25" s="10"/>
     </row>
     <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
@@ -1605,9 +1624,9 @@
         <v>11</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D26" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D26" s="9" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1621,7 +1640,7 @@
       <c r="C27" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D27" s="13"/>
+      <c r="D27" s="10"/>
     </row>
     <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
@@ -1631,9 +1650,9 @@
         <v>11</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D28" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D28" s="9" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1647,7 +1666,7 @@
       <c r="C29" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D29" s="13"/>
+      <c r="D29" s="10"/>
     </row>
     <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
@@ -1657,9 +1676,9 @@
         <v>18</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D30" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D30" s="9" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1673,7 +1692,7 @@
       <c r="C31" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D31" s="12"/>
+      <c r="D31" s="11"/>
     </row>
     <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
@@ -1685,7 +1704,7 @@
       <c r="C32" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D32" s="12"/>
+      <c r="D32" s="11"/>
     </row>
     <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
@@ -1697,7 +1716,7 @@
       <c r="C33" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D33" s="13"/>
+      <c r="D33" s="10"/>
     </row>
     <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
@@ -1707,9 +1726,9 @@
         <v>18</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D34" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D34" s="9" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1723,7 +1742,7 @@
       <c r="C35" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D35" s="12"/>
+      <c r="D35" s="11"/>
     </row>
     <row r="36" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
@@ -1735,7 +1754,7 @@
       <c r="C36" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D36" s="12"/>
+      <c r="D36" s="11"/>
     </row>
     <row r="37" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
@@ -1747,7 +1766,7 @@
       <c r="C37" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D37" s="13"/>
+      <c r="D37" s="10"/>
     </row>
     <row r="38" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
@@ -1757,7 +1776,7 @@
         <v>28</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>14</v>
@@ -1782,10 +1801,10 @@
         <v>1</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>94</v>
+        <v>72</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>14</v>
@@ -1796,10 +1815,10 @@
         <v>1</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>96</v>
+        <v>74</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>14</v>
@@ -1807,12 +1826,12 @@
     </row>
     <row r="42" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="43" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="16" t="s">
+      <c r="A43" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B43" s="16"/>
-      <c r="C43" s="16"/>
-      <c r="D43" s="16"/>
+      <c r="B43" s="12"/>
+      <c r="C43" s="12"/>
+      <c r="D43" s="12"/>
     </row>
     <row r="44" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
@@ -1825,7 +1844,7 @@
         <v>6</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1892,7 +1911,7 @@
         <v>37</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D49" s="3" t="s">
         <v>14</v>
@@ -1921,9 +1940,9 @@
         <v>40</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="D51" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D51" s="14" t="s">
         <v>16</v>
       </c>
       <c r="J51" s="6"/>
@@ -1936,9 +1955,9 @@
         <v>41</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D52" s="14"/>
+        <v>43</v>
+      </c>
+      <c r="D52" s="15"/>
       <c r="J52" s="6"/>
     </row>
     <row r="53" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1949,18 +1968,18 @@
         <v>42</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D53" s="10"/>
+        <v>44</v>
+      </c>
+      <c r="D53" s="16"/>
     </row>
     <row r="54" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="55" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="16" t="s">
-        <v>97</v>
-      </c>
-      <c r="B55" s="16"/>
-      <c r="C55" s="16"/>
-      <c r="D55" s="16"/>
+      <c r="A55" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="B55" s="12"/>
+      <c r="C55" s="12"/>
+      <c r="D55" s="12"/>
     </row>
     <row r="56" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="4" t="s">
@@ -1973,7 +1992,7 @@
         <v>6</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="57" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1981,10 +2000,10 @@
         <v>1</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>101</v>
+        <v>79</v>
       </c>
       <c r="D57" s="3" t="s">
         <v>14</v>
@@ -1995,10 +2014,10 @@
         <v>1</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>99</v>
+        <v>77</v>
       </c>
       <c r="D58" s="3" t="s">
         <v>14</v>
@@ -2009,10 +2028,10 @@
         <v>1</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>103</v>
+        <v>81</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>102</v>
+        <v>80</v>
       </c>
       <c r="D59" s="3" t="s">
         <v>14</v>
@@ -2023,10 +2042,10 @@
         <v>3</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>105</v>
+        <v>83</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>104</v>
+        <v>82</v>
       </c>
       <c r="D60" s="3" t="s">
         <v>14</v>
@@ -2037,10 +2056,10 @@
         <v>1</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>106</v>
+        <v>84</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>107</v>
+        <v>85</v>
       </c>
       <c r="D61" s="3" t="s">
         <v>14</v>
@@ -2051,10 +2070,10 @@
         <v>1</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>108</v>
+        <v>86</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>109</v>
+        <v>87</v>
       </c>
       <c r="D62" s="3" t="s">
         <v>14</v>
@@ -2065,10 +2084,10 @@
         <v>3</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>110</v>
+        <v>88</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>111</v>
+        <v>89</v>
       </c>
       <c r="D63" s="3" t="s">
         <v>14</v>
@@ -2079,25 +2098,25 @@
         <v>1</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>200</v>
+        <v>178</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>201</v>
+        <v>179</v>
       </c>
       <c r="D64" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="66" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="B66" s="16"/>
-      <c r="C66" s="16"/>
-      <c r="D66" s="16"/>
-    </row>
-    <row r="67" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="66" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="B66" s="12"/>
+      <c r="C66" s="12"/>
+      <c r="D66" s="12"/>
+    </row>
+    <row r="67" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="4" t="s">
         <v>4</v>
       </c>
@@ -2108,596 +2127,601 @@
         <v>1</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="2">
         <v>8</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>68</v>
+        <v>181</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>202</v>
-      </c>
-      <c r="D68" s="15" t="s">
+        <v>210</v>
+      </c>
+      <c r="D68" s="14" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E68" s="19"/>
+    </row>
+    <row r="69" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="2">
-        <f>9*4+13*4+4+4+4</f>
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>44</v>
+        <v>182</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
       <c r="D69" s="15"/>
-    </row>
-    <row r="70" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E69" s="19"/>
+    </row>
+    <row r="70" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="2">
-        <f>42+16*2+13*2+2+2+2</f>
-        <v>106</v>
+        <v>67</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>65</v>
+        <v>183</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>202</v>
+        <v>210</v>
       </c>
       <c r="D70" s="15"/>
-    </row>
-    <row r="71" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E70" s="19"/>
+    </row>
+    <row r="71" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="2">
-        <f>28</f>
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>65</v>
+        <v>183</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>203</v>
+        <v>211</v>
       </c>
       <c r="D71" s="15"/>
-    </row>
-    <row r="72" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E71" s="19"/>
+    </row>
+    <row r="72" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="2">
-        <f>7+4*4+2</f>
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>66</v>
+        <v>184</v>
       </c>
       <c r="C72" s="5" t="s">
-        <v>202</v>
+        <v>210</v>
       </c>
       <c r="D72" s="15"/>
-    </row>
-    <row r="73" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E72" s="19"/>
+    </row>
+    <row r="73" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="2">
-        <f>2*5+4</f>
         <v>14</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>66</v>
+        <v>184</v>
       </c>
       <c r="C73" s="5" t="s">
-        <v>203</v>
+        <v>211</v>
       </c>
       <c r="D73" s="15"/>
-    </row>
-    <row r="74" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E73" s="19"/>
+    </row>
+    <row r="74" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="2">
+        <v>2</v>
+      </c>
+      <c r="B74" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="C74" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="D74" s="15"/>
+      <c r="E74" s="19"/>
+    </row>
+    <row r="75" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="2">
         <f>11+4</f>
         <v>15</v>
       </c>
-      <c r="B74" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C74" s="5" t="s">
-        <v>202</v>
-      </c>
-      <c r="D74" s="15"/>
-    </row>
-    <row r="75" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="2">
+      <c r="B75" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="C75" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="D75" s="15"/>
+      <c r="E75" s="19"/>
+    </row>
+    <row r="76" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="2">
+        <v>6</v>
+      </c>
+      <c r="B76" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="C76" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="D76" s="15"/>
+      <c r="E76" s="19"/>
+    </row>
+    <row r="77" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="2">
         <f>2*4+4</f>
         <v>12</v>
       </c>
-      <c r="B75" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C75" s="5" t="s">
-        <v>202</v>
-      </c>
-      <c r="D75" s="15"/>
-    </row>
-    <row r="76" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="2">
+      <c r="B77" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="C77" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="D77" s="15"/>
+      <c r="E77" s="19"/>
+    </row>
+    <row r="78" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="2">
+        <v>6</v>
+      </c>
+      <c r="B78" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="C78" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="D78" s="15"/>
+      <c r="E78" s="19"/>
+    </row>
+    <row r="79" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="2">
         <f>2*4+2*5</f>
         <v>18</v>
       </c>
-      <c r="B76" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="C76" s="5" t="s">
-        <v>203</v>
-      </c>
-      <c r="D76" s="15"/>
-    </row>
-    <row r="77" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="2">
-        <f>6+2*4+2</f>
+      <c r="B79" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="C79" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="D79" s="15"/>
+      <c r="E79" s="19"/>
+    </row>
+    <row r="80" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="2">
+        <v>12</v>
+      </c>
+      <c r="B80" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="C80" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="D80" s="15"/>
+      <c r="E80" s="19"/>
+    </row>
+    <row r="81" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="2">
+        <v>20</v>
+      </c>
+      <c r="B81" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="C81" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="D81" s="15"/>
+      <c r="E81" s="19"/>
+    </row>
+    <row r="82" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="2">
+        <v>58</v>
+      </c>
+      <c r="B82" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="C82" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="D82" s="15"/>
+      <c r="E82" s="19"/>
+    </row>
+    <row r="83" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="2">
+        <v>4</v>
+      </c>
+      <c r="B83" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="C83" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="D83" s="15"/>
+      <c r="E83" s="19"/>
+    </row>
+    <row r="84" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="2">
         <v>16</v>
       </c>
-      <c r="B77" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="C77" s="8" t="s">
-        <v>202</v>
-      </c>
-      <c r="D77" s="15"/>
-    </row>
-    <row r="78" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="2">
-        <f>2+4+2+6*2+2*3</f>
-        <v>26</v>
-      </c>
-      <c r="B78" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="C78" s="5" t="s">
-        <v>203</v>
-      </c>
-      <c r="D78" s="15"/>
-    </row>
-    <row r="79" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="2">
-        <f>2*13+8*2+8*4</f>
-        <v>74</v>
-      </c>
-      <c r="B79" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="C79" s="5" t="s">
-        <v>203</v>
-      </c>
-      <c r="D79" s="15"/>
-    </row>
-    <row r="80" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="2">
-        <f>4*4+6</f>
-        <v>22</v>
-      </c>
-      <c r="B80" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="C80" s="5" t="s">
-        <v>203</v>
-      </c>
-      <c r="D80" s="15"/>
-    </row>
-    <row r="81" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="2">
-        <f>2</f>
-        <v>2</v>
-      </c>
-      <c r="B81" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="C81" s="5" t="s">
-        <v>202</v>
-      </c>
-      <c r="D81" s="15"/>
-    </row>
-    <row r="82" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="2">
+      <c r="B84" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="C84" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="D84" s="15"/>
+      <c r="E84" s="19"/>
+    </row>
+    <row r="85" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="2">
+        <v>4</v>
+      </c>
+      <c r="B85" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="C85" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="D85" s="15"/>
+      <c r="E85" s="19"/>
+    </row>
+    <row r="86" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="2">
         <f>5*2+8</f>
         <v>18</v>
       </c>
-      <c r="B82" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="C82" s="5" t="s">
-        <v>203</v>
-      </c>
-      <c r="D82" s="15"/>
-    </row>
-    <row r="83" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="2">
+      <c r="B86" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="C86" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="D86" s="15"/>
+      <c r="E86" s="19"/>
+    </row>
+    <row r="87" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A87" s="2">
         <f>2+4</f>
         <v>6</v>
       </c>
-      <c r="B83" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="C83" s="5" t="s">
-        <v>202</v>
-      </c>
-      <c r="D83" s="15"/>
-    </row>
-    <row r="84" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="2">
-        <f>4+2+2*4</f>
-        <v>14</v>
-      </c>
-      <c r="B84" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="C84" s="5" t="s">
-        <v>202</v>
-      </c>
-      <c r="D84" s="15"/>
-    </row>
-    <row r="85" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="2">
-        <f>2*6</f>
-        <v>12</v>
-      </c>
-      <c r="B85" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="C85" s="5" t="s">
-        <v>203</v>
-      </c>
-      <c r="D85" s="15"/>
-    </row>
-    <row r="86" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="2">
-        <f>4+2*4</f>
-        <v>12</v>
-      </c>
-      <c r="B86" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="C86" s="5" t="s">
-        <v>203</v>
-      </c>
-      <c r="D86" s="15"/>
-    </row>
-    <row r="87" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="2">
+      <c r="B87" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="C87" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="D87" s="15"/>
+      <c r="E87" s="19"/>
+    </row>
+    <row r="88" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="2">
+        <v>8</v>
+      </c>
+      <c r="B88" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="C88" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="D88" s="15"/>
+      <c r="E88" s="19"/>
+    </row>
+    <row r="89" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A89" s="2">
+        <v>4</v>
+      </c>
+      <c r="B89" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="C89" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="D89" s="15"/>
+      <c r="E89" s="19"/>
+    </row>
+    <row r="90" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A90" s="2">
         <f>4+4+4</f>
         <v>12</v>
       </c>
-      <c r="B87" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="C87" s="5" t="s">
-        <v>203</v>
-      </c>
-      <c r="D87" s="15"/>
-    </row>
-    <row r="88" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="2">
+      <c r="B90" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="C90" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="D90" s="15"/>
+      <c r="E90" s="19"/>
+    </row>
+    <row r="91" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A91" s="2">
+        <v>4</v>
+      </c>
+      <c r="B91" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="C91" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="D91" s="15"/>
+      <c r="E91" s="19"/>
+    </row>
+    <row r="92" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A92" s="2">
         <f>8+4+8</f>
         <v>20</v>
       </c>
-      <c r="B88" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="C88" s="5" t="s">
-        <v>203</v>
-      </c>
-      <c r="D88" s="15"/>
-    </row>
-    <row r="89" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="2">
+      <c r="B92" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="C92" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="D92" s="15"/>
+      <c r="E92" s="19"/>
+    </row>
+    <row r="93" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A93" s="2">
         <v>4</v>
       </c>
-      <c r="B89" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C89" s="5" t="s">
-        <v>203</v>
-      </c>
-      <c r="D89" s="15"/>
-    </row>
-    <row r="90" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="2">
-        <f>2+2*5</f>
-        <v>12</v>
-      </c>
-      <c r="B90" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="C90" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="D90" s="15"/>
-    </row>
-    <row r="91" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="2">
+      <c r="B93" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="C93" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="D93" s="15"/>
+      <c r="E93" s="19"/>
+    </row>
+    <row r="94" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A94" s="2">
+        <v>32</v>
+      </c>
+      <c r="B94" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="C94" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="D94" s="15"/>
+      <c r="E94" s="19"/>
+    </row>
+    <row r="95" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A95" s="2">
+        <v>13</v>
+      </c>
+      <c r="B95" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="C95" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="D95" s="15"/>
+      <c r="E95" s="19"/>
+    </row>
+    <row r="96" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A96" s="2">
+        <v>4</v>
+      </c>
+      <c r="B96" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C96" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D96" s="15"/>
+      <c r="E96" s="19"/>
+    </row>
+    <row r="97" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A97" s="2">
+        <v>8</v>
+      </c>
+      <c r="B97" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="C97" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D97" s="15"/>
+      <c r="E97" s="19"/>
+    </row>
+    <row r="98" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A98" s="2">
+        <v>16</v>
+      </c>
+      <c r="B98" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C98" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D98" s="15"/>
+      <c r="E98" s="19"/>
+    </row>
+    <row r="99" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A99" s="2">
         <f>14*2+4</f>
         <v>32</v>
       </c>
-      <c r="B91" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="C91" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="D91" s="15"/>
-    </row>
-    <row r="92" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="2">
+      <c r="B99" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C99" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D99" s="15"/>
+      <c r="E99" s="19"/>
+    </row>
+    <row r="100" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A100" s="2">
         <v>4</v>
       </c>
-      <c r="B92" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="C92" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="D92" s="15"/>
-    </row>
-    <row r="93" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="2">
-        <f>A76+4+4*4+2*13</f>
+      <c r="B100" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C100" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D100" s="16"/>
+      <c r="E100" s="19"/>
+    </row>
+    <row r="101" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A101" s="2">
+        <v>140</v>
+      </c>
+      <c r="B101" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C101" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D101" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E101" s="19"/>
+    </row>
+    <row r="102" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A102" s="2">
+        <v>76</v>
+      </c>
+      <c r="B102" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B93" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="C93" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="D93" s="3" t="s">
+      <c r="C102" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D102" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="94" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="2">
-        <f>A69+A71+2</f>
-        <v>130</v>
-      </c>
-      <c r="B94" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="C94" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="D94" s="3" t="s">
+      <c r="E102" s="19"/>
+    </row>
+    <row r="103" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A103" s="2">
+        <f>42</f>
+        <v>42</v>
+      </c>
+      <c r="B103" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="C103" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D103" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A95" s="2">
+      <c r="E103" s="19"/>
+    </row>
+    <row r="104" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A104" s="2">
         <f>8</f>
         <v>8</v>
       </c>
-      <c r="B95" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="C95" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="D95" s="3" t="s">
+      <c r="B104" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="C104" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D104" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="96" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A96" s="2">
-        <f>42</f>
-        <v>42</v>
-      </c>
-      <c r="B96" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C96" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="D96" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="98" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="16" t="s">
-        <v>134</v>
-      </c>
-      <c r="B98" s="16"/>
-      <c r="C98" s="16"/>
-      <c r="D98" s="16"/>
-    </row>
-    <row r="99" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="4" t="s">
+      <c r="E104" s="19"/>
+    </row>
+    <row r="105" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="106" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A106" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="B106" s="12"/>
+      <c r="C106" s="12"/>
+      <c r="D106" s="12"/>
+    </row>
+    <row r="107" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A107" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B99" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="C99" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="D99" s="4" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="2">
+      <c r="B107" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C107" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D107" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A108" s="2">
         <v>2</v>
       </c>
-      <c r="B100" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="C100" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="D100" s="5" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="2">
+      <c r="B108" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C108" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D108" s="5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A109" s="2">
         <v>4</v>
       </c>
-      <c r="B101" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="C101" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="D101" s="5" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A102" s="2">
+      <c r="B109" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C109" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D109" s="5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A110" s="2">
         <v>2</v>
       </c>
-      <c r="B102" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="C102" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="D102" s="5" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="2">
+      <c r="B110" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C110" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="D110" s="5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A111" s="2">
         <v>2</v>
       </c>
-      <c r="B103" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="C103" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="D103" s="5" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="2">
-        <v>1</v>
-      </c>
-      <c r="B104" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="C104" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="D104" s="5" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A105" s="2">
-        <v>1</v>
-      </c>
-      <c r="B105" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="C105" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="D105" s="5" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A106" s="2">
-        <v>1</v>
-      </c>
-      <c r="B106" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="C106" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="D106" s="5" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="2">
-        <v>1</v>
-      </c>
-      <c r="B107" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="C107" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="D107" s="5" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A108" s="2">
-        <v>1</v>
-      </c>
-      <c r="B108" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="C108" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="D108" s="5" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="2">
-        <v>1</v>
-      </c>
-      <c r="B109" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="C109" s="5" t="s">
-        <v>190</v>
-      </c>
-      <c r="D109" s="5" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A110" s="2">
-        <v>1</v>
-      </c>
-      <c r="B110" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="C110" s="5" t="s">
-        <v>190</v>
-      </c>
-      <c r="D110" s="5" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="2">
-        <v>4</v>
-      </c>
       <c r="B111" s="5" t="s">
-        <v>146</v>
+        <v>115</v>
       </c>
       <c r="C111" s="5" t="s">
-        <v>191</v>
+        <v>114</v>
       </c>
       <c r="D111" s="5" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" s="2">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B112" s="5" t="s">
-        <v>147</v>
+        <v>116</v>
       </c>
       <c r="C112" s="5" t="s">
-        <v>190</v>
+        <v>114</v>
       </c>
       <c r="D112" s="5" t="s">
-        <v>189</v>
+        <v>117</v>
       </c>
     </row>
     <row r="113" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2705,13 +2729,13 @@
         <v>1</v>
       </c>
       <c r="B113" s="5" t="s">
-        <v>148</v>
+        <v>118</v>
       </c>
       <c r="C113" s="5" t="s">
-        <v>191</v>
+        <v>114</v>
       </c>
       <c r="D113" s="5" t="s">
-        <v>189</v>
+        <v>117</v>
       </c>
     </row>
     <row r="114" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2719,41 +2743,41 @@
         <v>1</v>
       </c>
       <c r="B114" s="5" t="s">
-        <v>149</v>
+        <v>119</v>
       </c>
       <c r="C114" s="5" t="s">
-        <v>191</v>
+        <v>114</v>
       </c>
       <c r="D114" s="5" t="s">
-        <v>189</v>
+        <v>117</v>
       </c>
     </row>
     <row r="115" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115" s="2">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B115" s="5" t="s">
-        <v>192</v>
+        <v>120</v>
       </c>
       <c r="C115" s="5" t="s">
-        <v>191</v>
+        <v>114</v>
       </c>
       <c r="D115" s="5" t="s">
-        <v>189</v>
+        <v>117</v>
       </c>
     </row>
     <row r="116" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A116" s="2">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B116" s="5" t="s">
-        <v>193</v>
+        <v>121</v>
       </c>
       <c r="C116" s="5" t="s">
-        <v>191</v>
+        <v>114</v>
       </c>
       <c r="D116" s="5" t="s">
-        <v>189</v>
+        <v>117</v>
       </c>
     </row>
     <row r="117" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2761,55 +2785,55 @@
         <v>1</v>
       </c>
       <c r="B117" s="5" t="s">
-        <v>194</v>
+        <v>122</v>
       </c>
       <c r="C117" s="5" t="s">
-        <v>191</v>
+        <v>168</v>
       </c>
       <c r="D117" s="5" t="s">
-        <v>189</v>
+        <v>167</v>
       </c>
     </row>
     <row r="118" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A118" s="2">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="B118" s="5" t="s">
-        <v>150</v>
+        <v>123</v>
       </c>
       <c r="C118" s="5" t="s">
-        <v>191</v>
+        <v>168</v>
       </c>
       <c r="D118" s="5" t="s">
-        <v>189</v>
+        <v>167</v>
       </c>
     </row>
     <row r="119" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A119" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B119" s="5" t="s">
-        <v>151</v>
+        <v>124</v>
       </c>
       <c r="C119" s="5" t="s">
-        <v>191</v>
+        <v>169</v>
       </c>
       <c r="D119" s="5" t="s">
-        <v>189</v>
+        <v>167</v>
       </c>
     </row>
     <row r="120" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A120" s="2">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B120" s="5" t="s">
-        <v>152</v>
+        <v>125</v>
       </c>
       <c r="C120" s="5" t="s">
-        <v>191</v>
+        <v>168</v>
       </c>
       <c r="D120" s="5" t="s">
-        <v>189</v>
+        <v>167</v>
       </c>
     </row>
     <row r="121" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2817,13 +2841,13 @@
         <v>1</v>
       </c>
       <c r="B121" s="5" t="s">
-        <v>153</v>
+        <v>126</v>
       </c>
       <c r="C121" s="5" t="s">
-        <v>191</v>
+        <v>169</v>
       </c>
       <c r="D121" s="5" t="s">
-        <v>189</v>
+        <v>167</v>
       </c>
     </row>
     <row r="122" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2831,41 +2855,41 @@
         <v>1</v>
       </c>
       <c r="B122" s="5" t="s">
-        <v>154</v>
+        <v>127</v>
       </c>
       <c r="C122" s="5" t="s">
-        <v>191</v>
+        <v>169</v>
       </c>
       <c r="D122" s="5" t="s">
-        <v>189</v>
+        <v>167</v>
       </c>
     </row>
     <row r="123" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A123" s="2">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B123" s="5" t="s">
-        <v>155</v>
+        <v>170</v>
       </c>
       <c r="C123" s="5" t="s">
-        <v>191</v>
+        <v>169</v>
       </c>
       <c r="D123" s="5" t="s">
-        <v>189</v>
+        <v>167</v>
       </c>
     </row>
     <row r="124" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A124" s="2">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B124" s="5" t="s">
-        <v>156</v>
+        <v>171</v>
       </c>
       <c r="C124" s="5" t="s">
-        <v>191</v>
+        <v>169</v>
       </c>
       <c r="D124" s="5" t="s">
-        <v>189</v>
+        <v>167</v>
       </c>
     </row>
     <row r="125" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2873,27 +2897,27 @@
         <v>1</v>
       </c>
       <c r="B125" s="5" t="s">
-        <v>157</v>
+        <v>172</v>
       </c>
       <c r="C125" s="5" t="s">
-        <v>191</v>
+        <v>169</v>
       </c>
       <c r="D125" s="5" t="s">
-        <v>189</v>
+        <v>167</v>
       </c>
     </row>
     <row r="126" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A126" s="2">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="B126" s="5" t="s">
-        <v>158</v>
+        <v>128</v>
       </c>
       <c r="C126" s="5" t="s">
-        <v>191</v>
+        <v>169</v>
       </c>
       <c r="D126" s="5" t="s">
-        <v>189</v>
+        <v>167</v>
       </c>
     </row>
     <row r="127" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2901,13 +2925,13 @@
         <v>1</v>
       </c>
       <c r="B127" s="5" t="s">
-        <v>159</v>
+        <v>129</v>
       </c>
       <c r="C127" s="5" t="s">
-        <v>191</v>
+        <v>169</v>
       </c>
       <c r="D127" s="5" t="s">
-        <v>189</v>
+        <v>167</v>
       </c>
     </row>
     <row r="128" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2915,27 +2939,27 @@
         <v>1</v>
       </c>
       <c r="B128" s="5" t="s">
-        <v>160</v>
+        <v>130</v>
       </c>
       <c r="C128" s="5" t="s">
-        <v>191</v>
+        <v>169</v>
       </c>
       <c r="D128" s="5" t="s">
-        <v>189</v>
+        <v>167</v>
       </c>
     </row>
     <row r="129" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A129" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B129" s="5" t="s">
-        <v>161</v>
+        <v>131</v>
       </c>
       <c r="C129" s="5" t="s">
-        <v>190</v>
+        <v>169</v>
       </c>
       <c r="D129" s="5" t="s">
-        <v>189</v>
+        <v>167</v>
       </c>
     </row>
     <row r="130" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2943,13 +2967,13 @@
         <v>1</v>
       </c>
       <c r="B130" s="5" t="s">
-        <v>162</v>
+        <v>132</v>
       </c>
       <c r="C130" s="5" t="s">
-        <v>191</v>
+        <v>169</v>
       </c>
       <c r="D130" s="5" t="s">
-        <v>189</v>
+        <v>167</v>
       </c>
     </row>
     <row r="131" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2957,13 +2981,13 @@
         <v>1</v>
       </c>
       <c r="B131" s="5" t="s">
-        <v>163</v>
+        <v>133</v>
       </c>
       <c r="C131" s="5" t="s">
-        <v>191</v>
+        <v>169</v>
       </c>
       <c r="D131" s="5" t="s">
-        <v>189</v>
+        <v>167</v>
       </c>
     </row>
     <row r="132" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2971,13 +2995,13 @@
         <v>1</v>
       </c>
       <c r="B132" s="5" t="s">
-        <v>164</v>
+        <v>134</v>
       </c>
       <c r="C132" s="5" t="s">
-        <v>191</v>
+        <v>169</v>
       </c>
       <c r="D132" s="5" t="s">
-        <v>189</v>
+        <v>167</v>
       </c>
     </row>
     <row r="133" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2985,13 +3009,13 @@
         <v>1</v>
       </c>
       <c r="B133" s="5" t="s">
-        <v>165</v>
+        <v>135</v>
       </c>
       <c r="C133" s="5" t="s">
-        <v>191</v>
+        <v>169</v>
       </c>
       <c r="D133" s="5" t="s">
-        <v>189</v>
+        <v>167</v>
       </c>
     </row>
     <row r="134" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2999,13 +3023,13 @@
         <v>1</v>
       </c>
       <c r="B134" s="5" t="s">
-        <v>166</v>
+        <v>136</v>
       </c>
       <c r="C134" s="5" t="s">
-        <v>190</v>
+        <v>169</v>
       </c>
       <c r="D134" s="5" t="s">
-        <v>189</v>
+        <v>167</v>
       </c>
     </row>
     <row r="135" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3013,13 +3037,13 @@
         <v>1</v>
       </c>
       <c r="B135" s="5" t="s">
-        <v>167</v>
+        <v>137</v>
       </c>
       <c r="C135" s="5" t="s">
-        <v>190</v>
+        <v>169</v>
       </c>
       <c r="D135" s="5" t="s">
-        <v>189</v>
+        <v>167</v>
       </c>
     </row>
     <row r="136" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3027,27 +3051,27 @@
         <v>1</v>
       </c>
       <c r="B136" s="5" t="s">
-        <v>168</v>
+        <v>138</v>
       </c>
       <c r="C136" s="5" t="s">
-        <v>190</v>
+        <v>169</v>
       </c>
       <c r="D136" s="5" t="s">
-        <v>189</v>
+        <v>167</v>
       </c>
     </row>
     <row r="137" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A137" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B137" s="5" t="s">
-        <v>169</v>
+        <v>139</v>
       </c>
       <c r="C137" s="5" t="s">
-        <v>191</v>
+        <v>168</v>
       </c>
       <c r="D137" s="5" t="s">
-        <v>189</v>
+        <v>167</v>
       </c>
     </row>
     <row r="138" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3055,13 +3079,13 @@
         <v>1</v>
       </c>
       <c r="B138" s="5" t="s">
-        <v>170</v>
+        <v>140</v>
       </c>
       <c r="C138" s="5" t="s">
-        <v>191</v>
+        <v>169</v>
       </c>
       <c r="D138" s="5" t="s">
-        <v>189</v>
+        <v>167</v>
       </c>
     </row>
     <row r="139" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3069,13 +3093,13 @@
         <v>1</v>
       </c>
       <c r="B139" s="5" t="s">
-        <v>171</v>
+        <v>141</v>
       </c>
       <c r="C139" s="5" t="s">
-        <v>191</v>
+        <v>169</v>
       </c>
       <c r="D139" s="5" t="s">
-        <v>189</v>
+        <v>167</v>
       </c>
     </row>
     <row r="140" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3083,13 +3107,13 @@
         <v>1</v>
       </c>
       <c r="B140" s="5" t="s">
-        <v>172</v>
+        <v>142</v>
       </c>
       <c r="C140" s="5" t="s">
-        <v>190</v>
+        <v>169</v>
       </c>
       <c r="D140" s="5" t="s">
-        <v>189</v>
+        <v>167</v>
       </c>
     </row>
     <row r="141" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3097,13 +3121,13 @@
         <v>1</v>
       </c>
       <c r="B141" s="5" t="s">
-        <v>173</v>
+        <v>143</v>
       </c>
       <c r="C141" s="5" t="s">
-        <v>190</v>
+        <v>169</v>
       </c>
       <c r="D141" s="5" t="s">
-        <v>189</v>
+        <v>167</v>
       </c>
     </row>
     <row r="142" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3111,13 +3135,13 @@
         <v>1</v>
       </c>
       <c r="B142" s="5" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="C142" s="5" t="s">
-        <v>191</v>
+        <v>168</v>
       </c>
       <c r="D142" s="5" t="s">
-        <v>189</v>
+        <v>167</v>
       </c>
     </row>
     <row r="143" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3125,27 +3149,27 @@
         <v>1</v>
       </c>
       <c r="B143" s="5" t="s">
-        <v>175</v>
+        <v>145</v>
       </c>
       <c r="C143" s="5" t="s">
-        <v>191</v>
+        <v>168</v>
       </c>
       <c r="D143" s="5" t="s">
-        <v>189</v>
+        <v>167</v>
       </c>
     </row>
     <row r="144" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A144" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B144" s="5" t="s">
-        <v>176</v>
+        <v>146</v>
       </c>
       <c r="C144" s="5" t="s">
-        <v>191</v>
+        <v>168</v>
       </c>
       <c r="D144" s="5" t="s">
-        <v>189</v>
+        <v>167</v>
       </c>
     </row>
     <row r="145" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3153,13 +3177,13 @@
         <v>1</v>
       </c>
       <c r="B145" s="5" t="s">
-        <v>177</v>
+        <v>147</v>
       </c>
       <c r="C145" s="5" t="s">
-        <v>191</v>
+        <v>169</v>
       </c>
       <c r="D145" s="5" t="s">
-        <v>189</v>
+        <v>167</v>
       </c>
     </row>
     <row r="146" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3167,13 +3191,13 @@
         <v>1</v>
       </c>
       <c r="B146" s="5" t="s">
-        <v>178</v>
+        <v>148</v>
       </c>
       <c r="C146" s="5" t="s">
-        <v>191</v>
+        <v>169</v>
       </c>
       <c r="D146" s="5" t="s">
-        <v>189</v>
+        <v>167</v>
       </c>
     </row>
     <row r="147" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3181,13 +3205,13 @@
         <v>1</v>
       </c>
       <c r="B147" s="5" t="s">
-        <v>179</v>
+        <v>149</v>
       </c>
       <c r="C147" s="5" t="s">
-        <v>190</v>
+        <v>169</v>
       </c>
       <c r="D147" s="5" t="s">
-        <v>189</v>
+        <v>167</v>
       </c>
     </row>
     <row r="148" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3195,13 +3219,13 @@
         <v>1</v>
       </c>
       <c r="B148" s="5" t="s">
-        <v>180</v>
+        <v>150</v>
       </c>
       <c r="C148" s="5" t="s">
-        <v>190</v>
+        <v>168</v>
       </c>
       <c r="D148" s="5" t="s">
-        <v>189</v>
+        <v>167</v>
       </c>
     </row>
     <row r="149" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3209,13 +3233,13 @@
         <v>1</v>
       </c>
       <c r="B149" s="5" t="s">
-        <v>181</v>
+        <v>151</v>
       </c>
       <c r="C149" s="5" t="s">
-        <v>190</v>
+        <v>168</v>
       </c>
       <c r="D149" s="5" t="s">
-        <v>189</v>
+        <v>167</v>
       </c>
     </row>
     <row r="150" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3223,13 +3247,13 @@
         <v>1</v>
       </c>
       <c r="B150" s="5" t="s">
-        <v>182</v>
+        <v>152</v>
       </c>
       <c r="C150" s="5" t="s">
-        <v>190</v>
+        <v>169</v>
       </c>
       <c r="D150" s="5" t="s">
-        <v>189</v>
+        <v>167</v>
       </c>
     </row>
     <row r="151" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3237,27 +3261,27 @@
         <v>1</v>
       </c>
       <c r="B151" s="5" t="s">
-        <v>183</v>
+        <v>153</v>
       </c>
       <c r="C151" s="5" t="s">
-        <v>191</v>
+        <v>169</v>
       </c>
       <c r="D151" s="5" t="s">
-        <v>189</v>
+        <v>167</v>
       </c>
     </row>
     <row r="152" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A152" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B152" s="5" t="s">
-        <v>184</v>
+        <v>154</v>
       </c>
       <c r="C152" s="5" t="s">
-        <v>191</v>
+        <v>169</v>
       </c>
       <c r="D152" s="5" t="s">
-        <v>189</v>
+        <v>167</v>
       </c>
     </row>
     <row r="153" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3265,13 +3289,13 @@
         <v>1</v>
       </c>
       <c r="B153" s="5" t="s">
-        <v>185</v>
+        <v>155</v>
       </c>
       <c r="C153" s="5" t="s">
-        <v>190</v>
+        <v>169</v>
       </c>
       <c r="D153" s="5" t="s">
-        <v>189</v>
+        <v>167</v>
       </c>
     </row>
     <row r="154" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3279,13 +3303,13 @@
         <v>1</v>
       </c>
       <c r="B154" s="5" t="s">
-        <v>186</v>
+        <v>156</v>
       </c>
       <c r="C154" s="5" t="s">
-        <v>190</v>
+        <v>169</v>
       </c>
       <c r="D154" s="5" t="s">
-        <v>189</v>
+        <v>167</v>
       </c>
     </row>
     <row r="155" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3293,13 +3317,13 @@
         <v>1</v>
       </c>
       <c r="B155" s="5" t="s">
-        <v>187</v>
+        <v>157</v>
       </c>
       <c r="C155" s="5" t="s">
-        <v>190</v>
+        <v>168</v>
       </c>
       <c r="D155" s="5" t="s">
-        <v>189</v>
+        <v>167</v>
       </c>
     </row>
     <row r="156" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3307,36 +3331,55 @@
         <v>1</v>
       </c>
       <c r="B156" s="5" t="s">
-        <v>188</v>
+        <v>158</v>
       </c>
       <c r="C156" s="5" t="s">
-        <v>190</v>
+        <v>168</v>
       </c>
       <c r="D156" s="5" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="157" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+        <v>167</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A157" s="2">
+        <v>1</v>
+      </c>
+      <c r="B157" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="C157" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="D157" s="5" t="s">
+        <v>167</v>
+      </c>
+    </row>
     <row r="158" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A158" s="16" t="s">
-        <v>195</v>
-      </c>
-      <c r="B158" s="16"/>
-      <c r="C158" s="16"/>
-      <c r="D158" s="16"/>
+      <c r="A158" s="2">
+        <v>1</v>
+      </c>
+      <c r="B158" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="C158" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="D158" s="5" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="159" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A159" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B159" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="C159" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D159" s="4" t="s">
-        <v>64</v>
+      <c r="A159" s="2">
+        <v>1</v>
+      </c>
+      <c r="B159" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="C159" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="D159" s="5" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="160" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3344,13 +3387,13 @@
         <v>1</v>
       </c>
       <c r="B160" s="5" t="s">
-        <v>197</v>
+        <v>162</v>
       </c>
       <c r="C160" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="D160" s="9" t="s">
-        <v>16</v>
+        <v>169</v>
+      </c>
+      <c r="D160" s="5" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="161" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3358,33 +3401,126 @@
         <v>1</v>
       </c>
       <c r="B161" s="5" t="s">
-        <v>196</v>
+        <v>163</v>
       </c>
       <c r="C161" s="5" t="s">
-        <v>199</v>
-      </c>
-      <c r="D161" s="10"/>
+        <v>168</v>
+      </c>
+      <c r="D161" s="5" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A162" s="2">
+        <v>1</v>
+      </c>
+      <c r="B162" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="C162" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="D162" s="5" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A163" s="2">
+        <v>1</v>
+      </c>
+      <c r="B163" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C163" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="D163" s="5" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A164" s="2">
+        <v>1</v>
+      </c>
+      <c r="B164" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="C164" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="D164" s="5" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="166" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A166" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="B166" s="12"/>
+      <c r="C166" s="12"/>
+      <c r="D166" s="12"/>
+    </row>
+    <row r="167" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A167" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B167" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C167" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D167" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A168" s="2">
+        <v>1</v>
+      </c>
+      <c r="B168" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="C168" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="D168" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A169" s="2">
+        <v>1</v>
+      </c>
+      <c r="B169" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="C169" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="D169" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="D168:D169"/>
+    <mergeCell ref="D34:D37"/>
+    <mergeCell ref="D51:D53"/>
+    <mergeCell ref="D68:D100"/>
+    <mergeCell ref="A106:D106"/>
+    <mergeCell ref="A166:D166"/>
+    <mergeCell ref="A55:D55"/>
+    <mergeCell ref="A66:D66"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="D3:D8"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A22:D22"/>
+    <mergeCell ref="D14:D16"/>
     <mergeCell ref="D24:D25"/>
     <mergeCell ref="D26:D27"/>
     <mergeCell ref="D28:D29"/>
     <mergeCell ref="D30:D33"/>
     <mergeCell ref="A43:D43"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="D3:D8"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A22:D22"/>
-    <mergeCell ref="D14:D16"/>
-    <mergeCell ref="D160:D161"/>
-    <mergeCell ref="D34:D37"/>
-    <mergeCell ref="D51:D53"/>
-    <mergeCell ref="D68:D92"/>
-    <mergeCell ref="A98:D98"/>
-    <mergeCell ref="A158:D158"/>
-    <mergeCell ref="A55:D55"/>
-    <mergeCell ref="A66:D66"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D13" r:id="rId1" xr:uid="{DF9FA33A-53A5-4892-B518-93B78A977082}"/>
@@ -3397,10 +3533,10 @@
     <hyperlink ref="D48" r:id="rId8" xr:uid="{A051E3DE-AD94-48FD-92AE-0E754A369DB4}"/>
     <hyperlink ref="D49" r:id="rId9" xr:uid="{E610B6A5-9E79-4836-9C56-D528326DE1C5}"/>
     <hyperlink ref="D50" r:id="rId10" xr:uid="{0BAD72D1-AD4E-405C-9955-35E106B6C77A}"/>
-    <hyperlink ref="D93" r:id="rId11" xr:uid="{BCACB2B8-B0BD-41F9-BB52-1DB98E7C87F7}"/>
-    <hyperlink ref="D94" r:id="rId12" xr:uid="{086051CA-9FF2-4630-B881-36E716C2ADA3}"/>
-    <hyperlink ref="D95" r:id="rId13" xr:uid="{B47E111F-8B19-4982-8A16-B5A7925EA174}"/>
-    <hyperlink ref="D96" r:id="rId14" xr:uid="{4459086B-4ADA-4456-997A-303418702728}"/>
+    <hyperlink ref="D102" r:id="rId11" xr:uid="{BCACB2B8-B0BD-41F9-BB52-1DB98E7C87F7}"/>
+    <hyperlink ref="D101" r:id="rId12" xr:uid="{086051CA-9FF2-4630-B881-36E716C2ADA3}"/>
+    <hyperlink ref="D104" r:id="rId13" xr:uid="{B47E111F-8B19-4982-8A16-B5A7925EA174}"/>
+    <hyperlink ref="D103" r:id="rId14" xr:uid="{4459086B-4ADA-4456-997A-303418702728}"/>
     <hyperlink ref="D40" r:id="rId15" xr:uid="{C390AC12-F407-401C-A51B-52DBC149DC7D}"/>
     <hyperlink ref="D41" r:id="rId16" xr:uid="{96CFCFF2-C47E-42EB-9BBC-1E59DD4FC340}"/>
     <hyperlink ref="D58" r:id="rId17" location="nav-description" xr:uid="{3D6B3369-B93E-4DCF-8937-BDFFB41950CB}"/>

</xml_diff>